<commit_message>
Uppdatering Jon (ny data varsel)
</commit_message>
<xml_diff>
--- a/Data/varsel_bransch_manad.xlsx
+++ b/Data/varsel_bransch_manad.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">År</t>
   </si>
@@ -38,16 +38,22 @@
     <t xml:space="preserve">2023</t>
   </si>
   <si>
-    <t xml:space="preserve">Juli</t>
+    <t xml:space="preserve">Augusti</t>
   </si>
   <si>
     <t xml:space="preserve">Dalarnas län</t>
   </si>
   <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handel; reparation av motorfordon och motorcyklar</t>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tillverkning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Byggverksamhet</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,33 @@
         <v>11</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="n">
+        <v>11</v>
+      </c>
+      <c r="G3" t="n">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>